<commit_message>
1. Enhanced the Excel Reader function to read from test modules to test cases 2. Implemented new way of taking screenshot that will capture the test cases name when test fails.
</commit_message>
<xml_diff>
--- a/HybridTestAutomationFramework/src/Test Configurations And Data/POST.xlsx
+++ b/HybridTestAutomationFramework/src/Test Configurations And Data/POST.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="83">
   <si>
     <t>TCID</t>
   </si>
@@ -113,12 +113,6 @@
     <t>PAUSE</t>
   </si>
   <si>
-    <t>Pause execution for 1 seconds so that page loads completely.</t>
-  </si>
-  <si>
-    <t>https://redhat.invodx.com/social#feedpopup/All</t>
-  </si>
-  <si>
     <t>Validating that the POST button is there by Clicking on the POST Button</t>
   </si>
   <si>
@@ -140,9 +134,6 @@
     <t>Set the update text</t>
   </si>
   <si>
-    <t>//*[@id="statusUpdate"]/div[3]/button[2]</t>
-  </si>
-  <si>
     <t>Click</t>
   </si>
   <si>
@@ -180,6 +171,102 @@
   </si>
   <si>
     <t>//*[@id="statusUpdate"]/div[2]/div[1]/div[1]/div[1]/textarea</t>
+  </si>
+  <si>
+    <t>Pause execution for 5 seconds so that page loads completely.</t>
+  </si>
+  <si>
+    <t>XPATH</t>
+  </si>
+  <si>
+    <t>PARTIAL LINK</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>//button[text()='POST' and @class='post-status primary-btn']</t>
+  </si>
+  <si>
+    <t>Create New Ask for Help</t>
+  </si>
+  <si>
+    <t>Click on Ask for help</t>
+  </si>
+  <si>
+    <t>//*[@id="post-aq"]/a/i</t>
+  </si>
+  <si>
+    <t>Write the ask for help question.</t>
+  </si>
+  <si>
+    <t>SETTEXT</t>
+  </si>
+  <si>
+    <t>Xpath</t>
+  </si>
+  <si>
+    <t>//*[@id="postQuestion"]/div[2]/div[1]/div[1]/div[1]/textarea</t>
+  </si>
+  <si>
+    <t>Automation Testing: I want to know how to automate using Selenium with Maven and Java?</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>//button[text()='POST' and @class='ask-help-post primary-btn']</t>
+  </si>
+  <si>
+    <t>Create New Share an Idea</t>
+  </si>
+  <si>
+    <t>//*[@id="post-si"]/a/i</t>
+  </si>
+  <si>
+    <t>//*[@id="submitIdea"]/div[2]/div[1]/div[1]/div[1]/textarea</t>
+  </si>
+  <si>
+    <t>Enter an idea</t>
+  </si>
+  <si>
+    <t>//button[text()='POST' and @class='post-idea primary-btn']</t>
+  </si>
+  <si>
+    <t>Clicking on Post button</t>
+  </si>
+  <si>
+    <t>Click on Share an Idea on the pop-up</t>
+  </si>
+  <si>
+    <t>Create New Share Knowledge</t>
+  </si>
+  <si>
+    <t>Click on Share Knowledge on the pop-up</t>
+  </si>
+  <si>
+    <t>//*[@id="post-learning"]/a/i</t>
+  </si>
+  <si>
+    <t>//*[@id="shareKnowledge"]/div[2]/div[1]/div[1]/div[1]/textarea</t>
+  </si>
+  <si>
+    <t>Enter Knowledege text</t>
+  </si>
+  <si>
+    <t>Automation Testing: Let us plan for a diwali celebration in office</t>
+  </si>
+  <si>
+    <t>Automation Testing: Sun rises in the east &amp; sets in the west.</t>
+  </si>
+  <si>
+    <t>//button[text()='POST' and @class='post-knowledge primary-btn']</t>
   </si>
 </sst>
 </file>
@@ -379,7 +466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -445,48 +532,40 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="15" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -831,7 +910,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,32 +938,44 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="11" t="s">
+        <v>75</v>
+      </c>
       <c r="B5" s="27"/>
-      <c r="C5" s="11"/>
+      <c r="C5" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -919,27 +1010,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:M119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2:I19"/>
+      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="9.140625" style="2" collapsed="1"/>
     <col min="3" max="3" width="25" style="18" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="20.5703125" style="22" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.85546875" style="18" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.42578125" style="48" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" style="22" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.5703125" style="22" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="36.85546875" style="18" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.140625" style="42" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="17" style="2" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="6.42578125" style="40" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="5.28515625" style="38" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="13" width="9.140625" style="38" collapsed="1"/>
+    <col min="9" max="9" width="6.42578125" style="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="5.28515625" style="32" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="13" width="9.140625" style="32" collapsed="1"/>
     <col min="14" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
@@ -962,19 +1054,19 @@
       <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="36" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="34" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="15" t="s">
@@ -983,9 +1075,9 @@
       <c r="D2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="37"/>
+      <c r="E2" s="31"/>
       <c r="F2" s="15"/>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="37" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="9"/>
@@ -993,7 +1085,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="15" t="s">
@@ -1002,17 +1094,17 @@
       <c r="D3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="37"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="15"/>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="38" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="15" t="s">
@@ -1022,20 +1114,20 @@
         <v>25</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="38" t="s">
         <v>28</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="15" t="s">
@@ -1050,15 +1142,15 @@
       <c r="F5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="38" t="s">
         <v>29</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="15" t="s">
@@ -1073,243 +1165,253 @@
       <c r="F6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="44"/>
+      <c r="G6" s="39"/>
       <c r="H6" s="9"/>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="15" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="44"/>
+      <c r="G7" s="39">
+        <v>10</v>
+      </c>
       <c r="H7" s="9"/>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="15" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="44"/>
+        <v>26</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="39"/>
       <c r="H8" s="9"/>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="44" t="s">
-        <v>32</v>
+      <c r="G9" s="39">
+        <v>3</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="15" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="44"/>
+        <v>26</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="39"/>
       <c r="H10" s="9"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="44"/>
+      <c r="F11" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>49</v>
+      </c>
       <c r="H11" s="9"/>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" s="44" t="s">
-        <v>52</v>
-      </c>
+      <c r="F12" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="39"/>
       <c r="H12" s="9"/>
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="44"/>
+        <v>30</v>
+      </c>
+      <c r="E13" s="20"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="39">
+        <v>3</v>
+      </c>
       <c r="H13" s="9"/>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="15" t="s">
         <v>43</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
+        <v>42</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>49</v>
+      </c>
       <c r="H14" s="9"/>
       <c r="I14"/>
     </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="44" t="s">
+      <c r="F15" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="44" t="s">
-        <v>52</v>
-      </c>
+      <c r="G15" s="39"/>
       <c r="H15" s="9"/>
       <c r="I15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="15" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="44"/>
+        <v>30</v>
+      </c>
+      <c r="E16" s="20"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="39">
+        <v>3</v>
+      </c>
       <c r="H16" s="9"/>
       <c r="I16"/>
     </row>
     <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>23</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="44" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="G17" s="39" t="s">
+        <v>47</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="44"/>
+      <c r="G18" s="39"/>
       <c r="H18" s="9"/>
       <c r="I18"/>
     </row>
@@ -1320,409 +1422,1714 @@
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
       <c r="F19" s="15"/>
-      <c r="G19" s="43"/>
+      <c r="G19" s="37"/>
       <c r="H19" s="9"/>
       <c r="I19"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="51"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="47"/>
+    </row>
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B21" s="13"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
+      <c r="C21" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="16"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="39"/>
-      <c r="I21"/>
+      <c r="G21" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="33"/>
+      <c r="I21" t="s">
+        <v>65</v>
+      </c>
       <c r="J21"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
+      <c r="A22" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B22" s="13"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
+      <c r="C22" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="16"/>
       <c r="F22" s="16"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="39"/>
-      <c r="I22"/>
+      <c r="G22" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="33"/>
+      <c r="I22" t="s">
+        <v>65</v>
+      </c>
       <c r="J22"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
+      <c r="A23" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B23" s="13"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="39"/>
-      <c r="I23"/>
+      <c r="C23" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" s="33"/>
+      <c r="I23" t="s">
+        <v>65</v>
+      </c>
       <c r="J23"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
+      <c r="A24" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B24" s="13"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="39"/>
-      <c r="I24"/>
+      <c r="C24" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="33"/>
+      <c r="I24" t="s">
+        <v>65</v>
+      </c>
       <c r="J24"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
+      <c r="A25" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B25" s="13"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="16"/>
+      <c r="C25" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="G25" s="41"/>
-      <c r="H25" s="39"/>
-      <c r="I25"/>
+      <c r="H25" s="33"/>
+      <c r="I25" t="s">
+        <v>65</v>
+      </c>
       <c r="J25"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
+    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B26" s="13"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
+      <c r="C26" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="16"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="39"/>
-      <c r="I26"/>
+      <c r="G26" s="41">
+        <v>10</v>
+      </c>
+      <c r="H26" s="33"/>
+      <c r="I26" t="s">
+        <v>65</v>
+      </c>
       <c r="J26"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
+    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B27" s="13"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="16"/>
+      <c r="C27" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>54</v>
+      </c>
       <c r="G27" s="41"/>
-      <c r="H27" s="39"/>
-      <c r="I27"/>
+      <c r="H27" s="33"/>
+      <c r="I27" t="s">
+        <v>66</v>
+      </c>
       <c r="J27"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B28" s="13"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
+      <c r="C28" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="16"/>
       <c r="F28" s="16"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="39"/>
-      <c r="I28"/>
+      <c r="G28" s="41">
+        <v>3</v>
+      </c>
+      <c r="H28" s="33"/>
+      <c r="I28" t="s">
+        <v>65</v>
+      </c>
       <c r="J28"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
+      <c r="A29" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B29" s="13"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="16"/>
+      <c r="C29" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="G29" s="41"/>
-      <c r="H29" s="39"/>
-      <c r="I29"/>
+      <c r="H29" s="33"/>
+      <c r="I29" t="s">
+        <v>66</v>
+      </c>
       <c r="J29"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B30" s="13"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="C30" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="16"/>
       <c r="F30" s="16"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="39"/>
-      <c r="I30"/>
+      <c r="G30" s="41">
+        <v>3</v>
+      </c>
+      <c r="H30" s="33"/>
+      <c r="I30" t="s">
+        <v>65</v>
+      </c>
       <c r="J30"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
+    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B31" s="13"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="39"/>
-      <c r="I31"/>
+      <c r="C31" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" s="33"/>
+      <c r="I31" t="s">
+        <v>66</v>
+      </c>
       <c r="J31"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B32" s="13"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="16"/>
+      <c r="C32" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>67</v>
+      </c>
       <c r="G32" s="41"/>
-      <c r="H32" s="39"/>
-      <c r="I32"/>
+      <c r="H32" s="33"/>
+      <c r="I32" t="s">
+        <v>66</v>
+      </c>
       <c r="J32"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
+    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B33" s="13"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
+      <c r="C33" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="16"/>
       <c r="F33" s="16"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="39"/>
-      <c r="I33"/>
+      <c r="G33" s="41">
+        <v>3</v>
+      </c>
+      <c r="H33" s="33"/>
+      <c r="I33" t="s">
+        <v>65</v>
+      </c>
       <c r="J33"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
+    <row r="34" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B34" s="13"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="39"/>
-      <c r="I34"/>
+      <c r="C34" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G34" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="H34" s="33"/>
+      <c r="I34" t="s">
+        <v>65</v>
+      </c>
       <c r="J34"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="49"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="51"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="34"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="34"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="34"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="34"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="34"/>
+      <c r="A35" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="41"/>
+      <c r="H35" s="33"/>
+      <c r="I35" t="s">
+        <v>65</v>
+      </c>
+      <c r="J35"/>
+    </row>
+    <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="41">
+        <v>3</v>
+      </c>
+      <c r="H36" s="33"/>
+      <c r="I36" t="s">
+        <v>65</v>
+      </c>
+      <c r="J36"/>
+    </row>
+    <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H37" s="33"/>
+      <c r="I37" t="s">
+        <v>65</v>
+      </c>
+      <c r="J37"/>
+    </row>
+    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="33"/>
+      <c r="I38"/>
+      <c r="J38"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="35"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="34"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="33"/>
+      <c r="I39"/>
+      <c r="J39"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="35"/>
+      <c r="A40" s="45"/>
+      <c r="B40" s="46"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
       <c r="G40" s="46"/>
-      <c r="H40" s="34"/>
+      <c r="H40" s="47"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="46"/>
-      <c r="H41" s="34"/>
+      <c r="A41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="3"/>
+      <c r="I41" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="34"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="34"/>
+      <c r="A42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="3"/>
+      <c r="I42" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="46"/>
-      <c r="H43" s="34"/>
+      <c r="A43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="H43" s="3"/>
+      <c r="I43" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="46"/>
-      <c r="H44" s="34"/>
+      <c r="A44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="H44" s="3"/>
+      <c r="I44" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="49"/>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="51"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="31"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="47"/>
-      <c r="H47" s="31"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="31"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="47"/>
-      <c r="H49" s="31"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="31"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="47"/>
-      <c r="H50" s="31"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="31"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="31"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="31"/>
-      <c r="B52" s="31"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="31"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
-      <c r="B53" s="31"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="47"/>
-      <c r="H53" s="31"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="31"/>
-      <c r="B54" s="31"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="47"/>
-      <c r="H54" s="31"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="49"/>
-      <c r="B55" s="50"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="51"/>
+      <c r="A45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G45" s="44"/>
+      <c r="H45" s="3"/>
+      <c r="I45" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="44">
+        <v>10</v>
+      </c>
+      <c r="H46" s="3"/>
+      <c r="I46" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G47" s="44"/>
+      <c r="H47" s="3"/>
+      <c r="I47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="44">
+        <v>3</v>
+      </c>
+      <c r="H48" s="3"/>
+      <c r="I48" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F49" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G49" s="44"/>
+      <c r="H49" s="3"/>
+      <c r="I49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="44">
+        <v>3</v>
+      </c>
+      <c r="H50" s="3"/>
+      <c r="I50" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D51" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="F51" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G51" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="H51" s="3"/>
+      <c r="I51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="F52" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="G52" s="44"/>
+      <c r="H52" s="3"/>
+      <c r="I52" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="44">
+        <v>3</v>
+      </c>
+      <c r="H53" s="3"/>
+      <c r="I53" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F54" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G54" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="H54" s="3"/>
+      <c r="I54" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="F55" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="G55" s="44"/>
+      <c r="H55" s="3"/>
+      <c r="I55" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44">
+        <v>3</v>
+      </c>
+      <c r="H56" s="3"/>
+      <c r="I56" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D57" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="E57" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="F57" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="G57" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="H57" s="3"/>
+      <c r="I57" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="44"/>
+      <c r="H58" s="3"/>
+      <c r="I58" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="43"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="44"/>
+      <c r="H59" s="3"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="45"/>
+      <c r="B60" s="46"/>
+      <c r="C60" s="46"/>
+      <c r="D60" s="46"/>
+      <c r="E60" s="46"/>
+      <c r="F60" s="46"/>
+      <c r="G60" s="46"/>
+      <c r="H60" s="47"/>
+    </row>
+    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" s="13"/>
+      <c r="C61" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="40"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="H61" s="13"/>
+      <c r="I61" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" s="13"/>
+      <c r="C62" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" s="40"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="H62" s="13"/>
+      <c r="I62" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63" s="13"/>
+      <c r="C63" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E63" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="F63" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="G63" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="H63" s="13"/>
+      <c r="I63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64" s="13"/>
+      <c r="C64" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D64" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E64" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F64" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G64" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="H64" s="13"/>
+      <c r="I64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" s="13"/>
+      <c r="C65" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D65" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E65" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F65" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="G65" s="40"/>
+      <c r="H65" s="13"/>
+      <c r="I65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B66" s="13"/>
+      <c r="C66" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="D66" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="40">
+        <v>10</v>
+      </c>
+      <c r="H66" s="13"/>
+      <c r="I66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" s="13"/>
+      <c r="C67" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E67" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F67" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G67" s="40"/>
+      <c r="H67" s="13"/>
+      <c r="I67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" s="13"/>
+      <c r="C68" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E68" s="40"/>
+      <c r="F68" s="40"/>
+      <c r="G68" s="40">
+        <v>3</v>
+      </c>
+      <c r="H68" s="13"/>
+      <c r="I68" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" s="13"/>
+      <c r="C69" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D69" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="E69" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F69" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="G69" s="40"/>
+      <c r="H69" s="13"/>
+      <c r="I69" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70" s="13"/>
+      <c r="C70" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D70" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E70" s="40"/>
+      <c r="F70" s="40"/>
+      <c r="G70" s="40">
+        <v>3</v>
+      </c>
+      <c r="H70" s="13"/>
+      <c r="I70" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B71" s="13"/>
+      <c r="C71" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D71" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E71" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F71" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="G71" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="H71" s="13"/>
+      <c r="I71" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72" s="13"/>
+      <c r="C72" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D72" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F72" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G72" s="40"/>
+      <c r="H72" s="13"/>
+      <c r="I72" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" s="13"/>
+      <c r="C73" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E73" s="40"/>
+      <c r="F73" s="40"/>
+      <c r="G73" s="40">
+        <v>3</v>
+      </c>
+      <c r="H73" s="13"/>
+      <c r="I73" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" s="13"/>
+      <c r="C74" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D74" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E74" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F74" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="G74" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="H74" s="13"/>
+      <c r="I74" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" s="13"/>
+      <c r="C75" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D75" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E75" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F75" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="G75" s="40"/>
+      <c r="H75" s="13"/>
+      <c r="I75" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" s="13"/>
+      <c r="C76" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D76" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E76" s="40"/>
+      <c r="F76" s="40"/>
+      <c r="G76" s="40">
+        <v>3</v>
+      </c>
+      <c r="H76" s="13"/>
+      <c r="I76" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B77" s="13"/>
+      <c r="C77" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D77" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E77" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F77" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="G77" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="H77" s="13"/>
+      <c r="I77" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B78" s="13"/>
+      <c r="C78" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D78" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E78" s="40"/>
+      <c r="F78" s="40"/>
+      <c r="G78" s="40"/>
+      <c r="H78" s="13"/>
+      <c r="I78" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="13"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="16"/>
+      <c r="G79" s="40"/>
+      <c r="H79" s="13"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="45"/>
+      <c r="B80" s="46"/>
+      <c r="C80" s="46"/>
+      <c r="D80" s="46"/>
+      <c r="E80" s="46"/>
+      <c r="F80" s="46"/>
+      <c r="G80" s="46"/>
+      <c r="H80" s="47"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="44"/>
+      <c r="B81" s="44"/>
+      <c r="C81" s="44"/>
+      <c r="D81" s="44"/>
+      <c r="E81" s="44"/>
+      <c r="F81" s="44"/>
+      <c r="G81" s="44"/>
+      <c r="H81" s="44"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="44"/>
+      <c r="B82" s="44"/>
+      <c r="C82" s="44"/>
+      <c r="D82" s="44"/>
+      <c r="E82" s="44"/>
+      <c r="F82" s="44"/>
+      <c r="G82" s="44"/>
+      <c r="H82" s="44"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="44"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="44"/>
+      <c r="D83" s="44"/>
+      <c r="E83" s="44"/>
+      <c r="F83" s="44"/>
+      <c r="G83" s="44"/>
+      <c r="H83" s="44"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="44"/>
+      <c r="B84" s="44"/>
+      <c r="C84" s="44"/>
+      <c r="D84" s="44"/>
+      <c r="E84" s="44"/>
+      <c r="F84" s="44"/>
+      <c r="G84" s="44"/>
+      <c r="H84" s="44"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="44"/>
+      <c r="B85" s="44"/>
+      <c r="C85" s="44"/>
+      <c r="D85" s="44"/>
+      <c r="E85" s="44"/>
+      <c r="F85" s="44"/>
+      <c r="G85" s="44"/>
+      <c r="H85" s="44"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="44"/>
+      <c r="B86" s="44"/>
+      <c r="C86" s="44"/>
+      <c r="D86" s="44"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="44"/>
+      <c r="G86" s="44"/>
+      <c r="H86" s="44"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="44"/>
+      <c r="B87" s="44"/>
+      <c r="C87" s="44"/>
+      <c r="D87" s="44"/>
+      <c r="E87" s="44"/>
+      <c r="F87" s="44"/>
+      <c r="G87" s="44"/>
+      <c r="H87" s="44"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="44"/>
+      <c r="B88" s="44"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="44"/>
+      <c r="E88" s="44"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="44"/>
+      <c r="H88" s="44"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="44"/>
+      <c r="B89" s="44"/>
+      <c r="C89" s="44"/>
+      <c r="D89" s="44"/>
+      <c r="E89" s="44"/>
+      <c r="F89" s="44"/>
+      <c r="G89" s="44"/>
+      <c r="H89" s="44"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="44"/>
+      <c r="B90" s="44"/>
+      <c r="C90" s="44"/>
+      <c r="D90" s="44"/>
+      <c r="E90" s="44"/>
+      <c r="F90" s="44"/>
+      <c r="G90" s="44"/>
+      <c r="H90" s="44"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="44"/>
+      <c r="B91" s="44"/>
+      <c r="C91" s="44"/>
+      <c r="D91" s="44"/>
+      <c r="E91" s="44"/>
+      <c r="F91" s="44"/>
+      <c r="G91" s="44"/>
+      <c r="H91" s="44"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="44"/>
+      <c r="B92" s="44"/>
+      <c r="C92" s="44"/>
+      <c r="D92" s="44"/>
+      <c r="E92" s="44"/>
+      <c r="F92" s="44"/>
+      <c r="G92" s="44"/>
+      <c r="H92" s="44"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="44"/>
+      <c r="B93" s="44"/>
+      <c r="C93" s="44"/>
+      <c r="D93" s="44"/>
+      <c r="E93" s="44"/>
+      <c r="F93" s="44"/>
+      <c r="G93" s="44"/>
+      <c r="H93" s="44"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="44"/>
+      <c r="B94" s="44"/>
+      <c r="C94" s="44"/>
+      <c r="D94" s="44"/>
+      <c r="E94" s="44"/>
+      <c r="F94" s="44"/>
+      <c r="G94" s="44"/>
+      <c r="H94" s="44"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="44"/>
+      <c r="B95" s="44"/>
+      <c r="C95" s="44"/>
+      <c r="D95" s="44"/>
+      <c r="E95" s="44"/>
+      <c r="F95" s="44"/>
+      <c r="G95" s="44"/>
+      <c r="H95" s="44"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="44"/>
+      <c r="B96" s="44"/>
+      <c r="C96" s="44"/>
+      <c r="D96" s="44"/>
+      <c r="E96" s="44"/>
+      <c r="F96" s="44"/>
+      <c r="G96" s="44"/>
+      <c r="H96" s="44"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="44"/>
+      <c r="B97" s="44"/>
+      <c r="C97" s="44"/>
+      <c r="D97" s="44"/>
+      <c r="E97" s="44"/>
+      <c r="F97" s="44"/>
+      <c r="G97" s="44"/>
+      <c r="H97" s="44"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="44"/>
+      <c r="B98" s="44"/>
+      <c r="C98" s="44"/>
+      <c r="D98" s="44"/>
+      <c r="E98" s="44"/>
+      <c r="F98" s="44"/>
+      <c r="G98" s="44"/>
+      <c r="H98" s="44"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="44"/>
+      <c r="B99" s="44"/>
+      <c r="C99" s="44"/>
+      <c r="D99" s="44"/>
+      <c r="E99" s="44"/>
+      <c r="F99" s="44"/>
+      <c r="G99" s="44"/>
+      <c r="H99" s="44"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="44"/>
+      <c r="B100" s="44"/>
+      <c r="C100" s="44"/>
+      <c r="D100" s="44"/>
+      <c r="E100" s="44"/>
+      <c r="F100" s="44"/>
+      <c r="G100" s="44"/>
+      <c r="H100" s="44"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="44"/>
+      <c r="B101" s="44"/>
+      <c r="C101" s="44"/>
+      <c r="D101" s="44"/>
+      <c r="E101" s="44"/>
+      <c r="F101" s="44"/>
+      <c r="G101" s="44"/>
+      <c r="H101" s="44"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="44"/>
+      <c r="B102" s="44"/>
+      <c r="C102" s="44"/>
+      <c r="D102" s="44"/>
+      <c r="E102" s="44"/>
+      <c r="F102" s="44"/>
+      <c r="G102" s="44"/>
+      <c r="H102" s="44"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="44"/>
+      <c r="B103" s="44"/>
+      <c r="C103" s="44"/>
+      <c r="D103" s="44"/>
+      <c r="E103" s="44"/>
+      <c r="F103" s="44"/>
+      <c r="G103" s="44"/>
+      <c r="H103" s="44"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="44"/>
+      <c r="B104" s="44"/>
+      <c r="C104" s="44"/>
+      <c r="D104" s="44"/>
+      <c r="E104" s="44"/>
+      <c r="F104" s="44"/>
+      <c r="G104" s="44"/>
+      <c r="H104" s="44"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="44"/>
+      <c r="B105" s="44"/>
+      <c r="C105" s="44"/>
+      <c r="D105" s="44"/>
+      <c r="E105" s="44"/>
+      <c r="F105" s="44"/>
+      <c r="G105" s="44"/>
+      <c r="H105" s="44"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="44"/>
+      <c r="B106" s="44"/>
+      <c r="C106" s="44"/>
+      <c r="D106" s="44"/>
+      <c r="E106" s="44"/>
+      <c r="F106" s="44"/>
+      <c r="G106" s="44"/>
+      <c r="H106" s="44"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="44"/>
+      <c r="B107" s="44"/>
+      <c r="C107" s="44"/>
+      <c r="D107" s="44"/>
+      <c r="E107" s="44"/>
+      <c r="F107" s="44"/>
+      <c r="G107" s="44"/>
+      <c r="H107" s="44"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="44"/>
+      <c r="B108" s="44"/>
+      <c r="C108" s="44"/>
+      <c r="D108" s="44"/>
+      <c r="E108" s="44"/>
+      <c r="F108" s="44"/>
+      <c r="G108" s="44"/>
+      <c r="H108" s="44"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="44"/>
+      <c r="B109" s="44"/>
+      <c r="C109" s="44"/>
+      <c r="D109" s="44"/>
+      <c r="E109" s="44"/>
+      <c r="F109" s="44"/>
+      <c r="G109" s="44"/>
+      <c r="H109" s="44"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="44"/>
+      <c r="B110" s="44"/>
+      <c r="C110" s="44"/>
+      <c r="D110" s="44"/>
+      <c r="E110" s="44"/>
+      <c r="F110" s="44"/>
+      <c r="G110" s="44"/>
+      <c r="H110" s="44"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="44"/>
+      <c r="B111" s="44"/>
+      <c r="C111" s="44"/>
+      <c r="D111" s="44"/>
+      <c r="E111" s="44"/>
+      <c r="F111" s="44"/>
+      <c r="G111" s="44"/>
+      <c r="H111" s="44"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="44"/>
+      <c r="B112" s="44"/>
+      <c r="C112" s="44"/>
+      <c r="D112" s="44"/>
+      <c r="E112" s="44"/>
+      <c r="F112" s="44"/>
+      <c r="G112" s="44"/>
+      <c r="H112" s="44"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="44"/>
+      <c r="B113" s="44"/>
+      <c r="C113" s="44"/>
+      <c r="D113" s="44"/>
+      <c r="E113" s="44"/>
+      <c r="F113" s="44"/>
+      <c r="G113" s="44"/>
+      <c r="H113" s="44"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="44"/>
+      <c r="B114" s="44"/>
+      <c r="C114" s="44"/>
+      <c r="D114" s="44"/>
+      <c r="E114" s="44"/>
+      <c r="F114" s="44"/>
+      <c r="G114" s="44"/>
+      <c r="H114" s="44"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="44"/>
+      <c r="B115" s="44"/>
+      <c r="C115" s="44"/>
+      <c r="D115" s="44"/>
+      <c r="E115" s="44"/>
+      <c r="F115" s="44"/>
+      <c r="G115" s="44"/>
+      <c r="H115" s="44"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="44"/>
+      <c r="B116" s="44"/>
+      <c r="C116" s="44"/>
+      <c r="D116" s="44"/>
+      <c r="E116" s="44"/>
+      <c r="F116" s="44"/>
+      <c r="G116" s="44"/>
+      <c r="H116" s="44"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="44"/>
+      <c r="B117" s="44"/>
+      <c r="C117" s="44"/>
+      <c r="D117" s="44"/>
+      <c r="E117" s="44"/>
+      <c r="F117" s="44"/>
+      <c r="G117" s="44"/>
+      <c r="H117" s="44"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="44"/>
+      <c r="B118" s="44"/>
+      <c r="C118" s="44"/>
+      <c r="D118" s="44"/>
+      <c r="E118" s="44"/>
+      <c r="F118" s="44"/>
+      <c r="G118" s="44"/>
+      <c r="H118" s="44"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="44"/>
+      <c r="B119" s="44"/>
+      <c r="C119" s="44"/>
+      <c r="D119" s="44"/>
+      <c r="E119" s="44"/>
+      <c r="F119" s="44"/>
+      <c r="G119" s="44"/>
+      <c r="H119" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="A55:H55"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="A80:H80"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="G9" r:id="rId1" location="feedpopup/All"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>